<commit_message>
updated mtow estimation sheet validation
</commit_message>
<xml_diff>
--- a/examples/0_analyses_of_ref_vehicle/4_mtow_estimation/estimate_mtow.xlsx
+++ b/examples/0_analyses_of_ref_vehicle/4_mtow_estimation/estimate_mtow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfiyandyhr/Github_Repos/MCEVS/examples/0_analyses_of_ref_vehicle/4_mtow_estimation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29A5AB0-FBA3-8A4A-AC52-58430893B6E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8919D10-A117-844F-B075-6B01EFF0F30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15320" yWindow="740" windowWidth="14920" windowHeight="18900" activeTab="5" xr2:uid="{843CD013-835A-1741-B375-CD508AE79BD2}"/>
   </bookViews>
@@ -15435,7 +15435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CE37D87-B951-4841-B7CA-13CC46090773}">
   <dimension ref="B1:AO56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -25264,8 +25264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3661B753-A267-5243-ABFD-E2825908B8D2}">
   <dimension ref="B1:CI136"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -44948,7 +44948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF2CC91-5E9A-2041-A25C-AEB7F568B05D}">
   <dimension ref="B1:AO81"/>
   <sheetViews>
-    <sheetView zoomScale="88" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="88" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -49270,8 +49270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3C31E77-07DC-9243-A410-566ED0D9F438}">
   <dimension ref="B1:AS82"/>
   <sheetViews>
-    <sheetView zoomScale="88" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="B1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -53748,7 +53748,7 @@
         <v>2814.1887475258045</v>
       </c>
       <c r="AL44" s="2">
-        <v>-3.5033735912293196E-9</v>
+        <v>-4.1245584725402296E-10</v>
       </c>
       <c r="AM44" s="2">
         <f t="shared" si="14"/>
@@ -53762,15 +53762,15 @@
         <v>2814.1887475298972</v>
       </c>
       <c r="AP44" s="2">
-        <v>-1.9581420929171145E-9</v>
+        <v>1.1332303984090686E-9</v>
       </c>
       <c r="AQ44" s="2">
         <f t="shared" si="10"/>
-        <v>6.8601032962003274E-18</v>
+        <v>-4.6740750410982637E-19</v>
       </c>
       <c r="AR44" s="2">
         <f t="shared" si="11"/>
-        <v>-5.2456994441739523E-18</v>
+        <v>3.035829775866579E-18</v>
       </c>
       <c r="AS44" s="2">
         <f t="shared" si="12"/>
@@ -55101,7 +55101,7 @@
   <dimension ref="B1:CI136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -66671,15 +66671,15 @@
         <v>680.14907836914062</v>
       </c>
       <c r="AL65" s="2">
-        <v>-0.4424282152140222</v>
+        <v>-2.5708698872676905E-2</v>
       </c>
       <c r="AM65" s="2">
         <f t="shared" si="40"/>
-        <v>-8.0805484189382895E-2</v>
+        <v>-4.6954597126694711E-3</v>
       </c>
       <c r="AN65" s="2">
         <f t="shared" si="41"/>
-        <v>0.10355699036039825</v>
+        <v>6.0175083545435807E-3</v>
       </c>
       <c r="AO65" s="2">
         <f t="shared" si="42"/>
@@ -66810,15 +66810,15 @@
         <v>680.13801574707031</v>
       </c>
       <c r="AL66" s="2">
-        <v>-0.33824579448355507</v>
+        <v>7.8466944136835082E-2</v>
       </c>
       <c r="AM66" s="2">
         <f t="shared" si="40"/>
-        <v>-6.1777513861868888E-2</v>
+        <v>1.4331272725838716E-2</v>
       </c>
       <c r="AN66" s="2">
         <f t="shared" si="41"/>
-        <v>8.6958592753270756E-3</v>
+        <v>-2.0172830382730539E-3</v>
       </c>
       <c r="AO66" s="2">
         <f t="shared" si="42"/>
@@ -66929,32 +66929,32 @@
       </c>
       <c r="AG67" s="2">
         <f t="shared" si="43"/>
-        <v>680.126953125</v>
+        <v>680.13801574707031</v>
       </c>
       <c r="AH67" s="2">
-        <v>0.18264089271588091</v>
+        <v>7.8466944136835082E-2</v>
       </c>
       <c r="AI67" s="2">
         <f t="shared" si="44"/>
-        <v>680.13801574707031</v>
+        <v>680.14907836914062</v>
       </c>
       <c r="AJ67" s="2">
-        <v>7.8466944136835082E-2</v>
+        <v>-2.5708698872676905E-2</v>
       </c>
       <c r="AK67" s="2">
         <f t="shared" si="39"/>
-        <v>680.13248443603516</v>
+        <v>680.14354705810547</v>
       </c>
       <c r="AL67" s="2">
-        <v>-0.39033679304566249</v>
+        <v>2.6379334434295743E-2</v>
       </c>
       <c r="AM67" s="2">
         <f t="shared" si="40"/>
-        <v>-7.1291460341713853E-2</v>
+        <v>2.0699057614227741E-3</v>
       </c>
       <c r="AN67" s="2">
         <f t="shared" si="41"/>
-        <v>-3.0628535334465357E-2</v>
+        <v>-6.7817836543294604E-4</v>
       </c>
       <c r="AO67" s="2">
         <f t="shared" si="42"/>
@@ -67065,36 +67065,36 @@
       </c>
       <c r="AG68" s="2">
         <f t="shared" si="43"/>
-        <v>680.126953125</v>
+        <v>680.14354705810547</v>
       </c>
       <c r="AH68" s="2">
-        <v>0.18264089271588091</v>
+        <v>2.6379334434295743E-2</v>
       </c>
       <c r="AI68" s="2">
         <f t="shared" si="44"/>
-        <v>680.13801574707031</v>
+        <v>680.14907836914062</v>
       </c>
       <c r="AJ68" s="2">
-        <v>0.13055413022857465</v>
+        <v>-2.5708698872676905E-2</v>
       </c>
       <c r="AK68" s="2">
         <f t="shared" si="39"/>
-        <v>680.13248443603516</v>
+        <v>680.14631271362305</v>
       </c>
       <c r="AL68" s="2">
-        <v>-0.41638245117746919</v>
+        <v>3.3537073068146128E-4</v>
       </c>
       <c r="AM68" s="2">
         <f t="shared" si="40"/>
-        <v>-7.6048462594279678E-2</v>
+        <v>8.846856664120395E-6</v>
       </c>
       <c r="AN68" s="2">
         <f t="shared" si="41"/>
-        <v>-5.4360448755916439E-2</v>
+        <v>-8.6219451257993133E-6</v>
       </c>
       <c r="AO68" s="2">
         <f t="shared" si="42"/>
-        <v>1.10626220703125E-2</v>
+        <v>5.53131103515625E-3</v>
       </c>
       <c r="BG68" s="2" t="s">
         <v>183</v>
@@ -67201,36 +67201,36 @@
       </c>
       <c r="AG69" s="2">
         <f t="shared" si="43"/>
-        <v>680.126953125</v>
+        <v>680.14631271362305</v>
       </c>
       <c r="AH69" s="2">
-        <v>0.18264089271588091</v>
+        <v>3.3537073068146128E-4</v>
       </c>
       <c r="AI69" s="2">
         <f t="shared" si="44"/>
-        <v>680.13801574707031</v>
+        <v>680.14907836914062</v>
       </c>
       <c r="AJ69" s="2">
-        <v>0.15659756442391881</v>
+        <v>-2.5708698872676905E-2</v>
       </c>
       <c r="AK69" s="2">
         <f t="shared" si="39"/>
-        <v>680.13248443603516</v>
+        <v>680.14769554138184</v>
       </c>
       <c r="AL69" s="2">
-        <v>-0.4033596088743252</v>
+        <v>-1.2686650833074964E-2</v>
       </c>
       <c r="AM69" s="2">
         <f t="shared" si="40"/>
-        <v>-7.3669959050335312E-2</v>
+        <v>-4.2547313597889198E-6</v>
       </c>
       <c r="AN69" s="2">
         <f t="shared" si="41"/>
-        <v>-6.316513233670383E-2</v>
+        <v>3.2615728597031984E-4</v>
       </c>
       <c r="AO69" s="2">
         <f t="shared" si="42"/>
-        <v>1.10626220703125E-2</v>
+        <v>2.765655517578125E-3</v>
       </c>
       <c r="BG69" s="2" t="s">
         <v>187</v>
@@ -67256,36 +67256,36 @@
       </c>
       <c r="AG70" s="2">
         <f t="shared" si="43"/>
-        <v>680.126953125</v>
+        <v>680.14631271362305</v>
       </c>
       <c r="AH70" s="2">
-        <v>0.18264089271588091</v>
+        <v>3.3537073068146128E-4</v>
       </c>
       <c r="AI70" s="2">
         <f t="shared" si="44"/>
-        <v>680.13801574707031</v>
+        <v>680.14769554138184</v>
       </c>
       <c r="AJ70" s="2">
-        <v>0.1696192418071405</v>
+        <v>-1.2686650833074964E-2</v>
       </c>
       <c r="AK70" s="2">
         <f t="shared" si="39"/>
-        <v>680.13248443603516</v>
+        <v>680.14700412750244</v>
       </c>
       <c r="AL70" s="2">
-        <v>-0.40987102671806497</v>
+        <v>-6.1756367417729052E-3</v>
       </c>
       <c r="AM70" s="2">
         <f t="shared" si="40"/>
-        <v>-7.4859210218162067E-2</v>
+        <v>-2.0711278065116581E-6</v>
       </c>
       <c r="AN70" s="2">
         <f t="shared" si="41"/>
-        <v>-6.9522012790632401E-2</v>
+        <v>7.834814701478159E-5</v>
       </c>
       <c r="AO70" s="2">
         <f t="shared" si="42"/>
-        <v>1.10626220703125E-2</v>
+        <v>1.3828277587890625E-3</v>
       </c>
       <c r="BG70" s="2" t="s">
         <v>188</v>
@@ -67340,36 +67340,36 @@
       </c>
       <c r="AG71" s="2">
         <f t="shared" si="43"/>
-        <v>680.126953125</v>
+        <v>680.14631271362305</v>
       </c>
       <c r="AH71" s="2">
-        <v>0.18264089271588091</v>
+        <v>3.3537073068146128E-4</v>
       </c>
       <c r="AI71" s="2">
         <f t="shared" si="44"/>
-        <v>680.13801574707031</v>
+        <v>680.14700412750244</v>
       </c>
       <c r="AJ71" s="2">
-        <v>0.17613007057207142</v>
+        <v>-6.1756367417729052E-3</v>
       </c>
       <c r="AK71" s="2">
         <f t="shared" si="39"/>
-        <v>680.13248443603516</v>
+        <v>680.14665842056274</v>
       </c>
       <c r="AL71" s="2">
-        <v>-0.41312673812080902</v>
+        <v>-2.9201321772234223E-3</v>
       </c>
       <c r="AM71" s="2">
         <f t="shared" si="40"/>
-        <v>-7.5453836255184509E-2</v>
+        <v>-9.7932686196186543E-7</v>
       </c>
       <c r="AN71" s="2">
         <f t="shared" si="41"/>
-        <v>-7.276404154042776E-2</v>
+        <v>1.8033675564494277E-5</v>
       </c>
       <c r="AO71" s="2">
         <f t="shared" si="42"/>
-        <v>1.10626220703125E-2</v>
+        <v>6.9141387939453125E-4</v>
       </c>
       <c r="BG71" s="2" t="s">
         <v>190</v>
@@ -67464,36 +67464,36 @@
       </c>
       <c r="AG72" s="2">
         <f t="shared" si="43"/>
-        <v>680.126953125</v>
+        <v>680.14631271362305</v>
       </c>
       <c r="AH72" s="2">
-        <v>0.18264089271588091</v>
+        <v>3.3537073068146128E-4</v>
       </c>
       <c r="AI72" s="2">
         <f t="shared" si="44"/>
-        <v>680.13801574707031</v>
+        <v>680.14665842056274</v>
       </c>
       <c r="AJ72" s="2">
-        <v>0.17938548247138897</v>
+        <v>-2.9201321772234223E-3</v>
       </c>
       <c r="AK72" s="2">
         <f t="shared" si="39"/>
-        <v>680.13248443603516</v>
+        <v>680.1464855670929</v>
       </c>
       <c r="AL72" s="2">
-        <v>-0.41149888221161746</v>
+        <v>-1.2923805156788148E-3</v>
       </c>
       <c r="AM72" s="2">
         <f t="shared" si="40"/>
-        <v>-7.5156523198716935E-2</v>
+        <v>-4.3342659786168786E-7</v>
       </c>
       <c r="AN72" s="2">
         <f t="shared" si="41"/>
-        <v>-7.3816925521968252E-2</v>
+        <v>3.7739219290503068E-6</v>
       </c>
       <c r="AO72" s="2">
         <f t="shared" si="42"/>
-        <v>1.10626220703125E-2</v>
+        <v>3.4570693969726562E-4</v>
       </c>
       <c r="BG72" s="2" t="s">
         <v>192</v>
@@ -67570,36 +67570,36 @@
       </c>
       <c r="AG73" s="2">
         <f t="shared" si="43"/>
-        <v>680.126953125</v>
+        <v>680.14631271362305</v>
       </c>
       <c r="AH73" s="2">
-        <v>0.18264089271588091</v>
+        <v>3.3537073068146128E-4</v>
       </c>
       <c r="AI73" s="2">
         <f t="shared" si="44"/>
-        <v>680.13801574707031</v>
+        <v>680.1464855670929</v>
       </c>
       <c r="AJ73" s="2">
-        <v>0.18101318779872599</v>
+        <v>-1.2923805156788148E-3</v>
       </c>
       <c r="AK73" s="2">
         <f t="shared" si="39"/>
-        <v>680.13248443603516</v>
+        <v>680.14639914035797</v>
       </c>
       <c r="AL73" s="2">
-        <v>-0.4106849544114084</v>
+        <v>-4.7850484088485246E-4</v>
       </c>
       <c r="AM73" s="2">
         <f t="shared" si="40"/>
-        <v>-7.5007866698680481E-2</v>
+        <v>-1.6047651812216935E-7</v>
       </c>
       <c r="AN73" s="2">
         <f t="shared" si="41"/>
-        <v>-7.4339392778983493E-2</v>
+        <v>6.1841033301757486E-7</v>
       </c>
       <c r="AO73" s="2">
         <f t="shared" si="42"/>
-        <v>1.10626220703125E-2</v>
+        <v>1.7285346984863281E-4</v>
       </c>
       <c r="BG73" s="2" t="s">
         <v>38</v>
@@ -67712,36 +67712,36 @@
       </c>
       <c r="AG74" s="2">
         <f t="shared" si="43"/>
-        <v>680.126953125</v>
+        <v>680.14631271362305</v>
       </c>
       <c r="AH74" s="2">
-        <v>0.18264089271588091</v>
+        <v>3.3537073068146128E-4</v>
       </c>
       <c r="AI74" s="2">
         <f t="shared" si="44"/>
-        <v>680.13801574707031</v>
+        <v>680.14639914035797</v>
       </c>
       <c r="AJ74" s="2">
-        <v>0.1818270403086899</v>
+        <v>-4.7850484088485246E-4</v>
       </c>
       <c r="AK74" s="2">
         <f t="shared" si="39"/>
-        <v>680.13248443603516</v>
+        <v>680.14635592699051</v>
       </c>
       <c r="AL74" s="2">
-        <v>-0.41109191829946212</v>
+        <v>-7.1567042141396087E-5</v>
       </c>
       <c r="AM74" s="2">
         <f t="shared" si="40"/>
-        <v>-7.5082194946497746E-2</v>
+        <v>-2.4001491215670939E-8</v>
       </c>
       <c r="AN74" s="2">
         <f t="shared" si="41"/>
-        <v>-7.4747626799212957E-2</v>
+        <v>3.4245176112468264E-8</v>
       </c>
       <c r="AO74" s="2">
         <f t="shared" si="42"/>
-        <v>1.10626220703125E-2</v>
+        <v>8.6426734924316406E-5</v>
       </c>
       <c r="BG74" s="2" t="s">
         <v>194</v>
@@ -67848,36 +67848,36 @@
       </c>
       <c r="AG75" s="2">
         <f t="shared" si="43"/>
-        <v>680.126953125</v>
+        <v>680.14631271362305</v>
       </c>
       <c r="AH75" s="2">
-        <v>0.18264089271588091</v>
+        <v>3.3537073068146128E-4</v>
       </c>
       <c r="AI75" s="2">
         <f t="shared" si="44"/>
-        <v>680.13801574707031</v>
+        <v>680.14635592699051</v>
       </c>
       <c r="AJ75" s="2">
-        <v>0.18223396652592783</v>
+        <v>-7.1567042141396087E-5</v>
       </c>
       <c r="AK75" s="2">
         <f t="shared" si="39"/>
-        <v>680.13248443603516</v>
+        <v>680.14633432030678</v>
       </c>
       <c r="AL75" s="2">
-        <v>-0.41129540025394817</v>
+        <v>1.3190184745326405E-4</v>
       </c>
       <c r="AM75" s="2">
         <f t="shared" si="40"/>
-        <v>-7.5119359072316649E-2</v>
+        <v>4.423601895863581E-8</v>
       </c>
       <c r="AN75" s="2">
         <f t="shared" si="41"/>
-        <v>-7.4951992202146073E-2</v>
+        <v>-9.4398250752157458E-9</v>
       </c>
       <c r="AO75" s="2">
         <f t="shared" si="42"/>
-        <v>1.10626220703125E-2</v>
+        <v>4.3213367462158203E-5</v>
       </c>
       <c r="BG75" s="2" t="s">
         <v>45</v>
@@ -67975,36 +67975,36 @@
       </c>
       <c r="AG76" s="2">
         <f t="shared" si="43"/>
-        <v>680.126953125</v>
+        <v>680.14633432030678</v>
       </c>
       <c r="AH76" s="2">
-        <v>0.18264089271588091</v>
+        <v>1.3190184745326405E-4</v>
       </c>
       <c r="AI76" s="2">
         <f t="shared" si="44"/>
-        <v>680.13801574707031</v>
+        <v>680.14635592699051</v>
       </c>
       <c r="AJ76" s="2">
-        <v>0.18243742962340548</v>
+        <v>-7.1567042141396087E-5</v>
       </c>
       <c r="AK76" s="2">
         <f t="shared" si="39"/>
-        <v>680.13248443603516</v>
+        <v>680.14634512364864</v>
       </c>
       <c r="AL76" s="2">
-        <v>-0.41119365927397666</v>
+        <v>3.0167404929670738E-5</v>
       </c>
       <c r="AM76" s="2">
         <f t="shared" si="40"/>
-        <v>-7.5100777008908867E-2</v>
+        <v>3.9791364430942761E-9</v>
       </c>
       <c r="AN76" s="2">
         <f t="shared" si="41"/>
-        <v>-7.5017114275386695E-2</v>
+        <v>-2.1589919398983058E-9</v>
       </c>
       <c r="AO76" s="2">
         <f t="shared" si="42"/>
-        <v>1.10626220703125E-2</v>
+        <v>2.1606683731079102E-5</v>
       </c>
       <c r="BG76" s="2" t="s">
         <v>197</v>
@@ -68106,36 +68106,36 @@
       </c>
       <c r="AG77" s="2">
         <f t="shared" si="43"/>
-        <v>680.126953125</v>
+        <v>680.14634512364864</v>
       </c>
       <c r="AH77" s="2">
-        <v>0.18264089271588091</v>
+        <v>3.0167404929670738E-5</v>
       </c>
       <c r="AI77" s="2">
         <f t="shared" si="44"/>
-        <v>680.13801574707031</v>
+        <v>680.14635592699051</v>
       </c>
       <c r="AJ77" s="2">
-        <v>0.18253916117191693</v>
+        <v>-7.1567042141396087E-5</v>
       </c>
       <c r="AK77" s="2">
         <f t="shared" si="39"/>
-        <v>680.13248443603516</v>
+        <v>680.14635052531958</v>
       </c>
       <c r="AL77" s="2">
-        <v>-0.4112445297623708</v>
+        <v>-2.0699817014246946E-5</v>
       </c>
       <c r="AM77" s="2">
         <f t="shared" si="40"/>
-        <v>-7.5110068040322053E-2</v>
+        <v>-6.2445976183887554E-10</v>
       </c>
       <c r="AN77" s="2">
         <f t="shared" si="41"/>
-        <v>-7.5068231499362592E-2</v>
+        <v>1.4814246765777989E-9</v>
       </c>
       <c r="AO77" s="2">
         <f t="shared" si="42"/>
-        <v>1.10626220703125E-2</v>
+        <v>1.0803341865539551E-5</v>
       </c>
       <c r="BG77" s="7" t="s">
         <v>199</v>
@@ -68238,36 +68238,36 @@
       </c>
       <c r="AG78" s="2">
         <f t="shared" si="43"/>
-        <v>680.126953125</v>
+        <v>680.14634512364864</v>
       </c>
       <c r="AH78" s="2">
-        <v>0.18264089271588091</v>
+        <v>3.0167404929670738E-5</v>
       </c>
       <c r="AI78" s="2">
         <f t="shared" si="44"/>
-        <v>680.13801574707031</v>
+        <v>680.14635052531958</v>
       </c>
       <c r="AJ78" s="2">
-        <v>0.18259002694367155</v>
+        <v>-2.0699817014246946E-5</v>
       </c>
       <c r="AK78" s="2">
         <f t="shared" si="39"/>
-        <v>680.13248443603516</v>
+        <v>680.14634782448411</v>
       </c>
       <c r="AL78" s="2">
-        <v>-0.41126996500679525</v>
+        <v>4.7337939577118959E-6</v>
       </c>
       <c r="AM78" s="2">
         <f t="shared" si="40"/>
-        <v>-7.511471355607019E-2</v>
+        <v>1.428062791759234E-10</v>
       </c>
       <c r="AN78" s="2">
         <f t="shared" si="41"/>
-        <v>-7.5093793991713592E-2</v>
+        <v>-9.7988668707784092E-11</v>
       </c>
       <c r="AO78" s="2">
         <f t="shared" si="42"/>
-        <v>1.10626220703125E-2</v>
+        <v>5.4016709327697754E-6</v>
       </c>
       <c r="BO78" s="2">
         <v>6</v>
@@ -68354,36 +68354,36 @@
       </c>
       <c r="AG79" s="2">
         <f t="shared" si="43"/>
-        <v>680.126953125</v>
+        <v>680.14634782448411</v>
       </c>
       <c r="AH79" s="2">
-        <v>0.18264089271588091</v>
+        <v>4.7337939577118959E-6</v>
       </c>
       <c r="AI79" s="2">
         <f t="shared" si="44"/>
-        <v>680.13801574707031</v>
+        <v>680.14635052531958</v>
       </c>
       <c r="AJ79" s="2">
-        <v>0.18261545982886673</v>
+        <v>-2.0699817014246946E-5</v>
       </c>
       <c r="AK79" s="5">
         <f t="shared" si="39"/>
-        <v>680.13248443603516</v>
+        <v>680.14634917490184</v>
       </c>
       <c r="AL79" s="2">
-        <v>-0.41128268262991696</v>
+        <v>-7.9830138020042796E-6</v>
       </c>
       <c r="AM79" s="2">
         <f t="shared" si="40"/>
-        <v>-7.5117036314110361E-2</v>
+        <v>-3.7789942500258528E-11</v>
       </c>
       <c r="AN79" s="2">
         <f t="shared" si="41"/>
-        <v>-7.5106576208112147E-2</v>
+        <v>1.6524692492369639E-10</v>
       </c>
       <c r="AO79" s="2">
         <f t="shared" si="42"/>
-        <v>1.10626220703125E-2</v>
+        <v>2.7008354663848877E-6</v>
       </c>
       <c r="BO79" s="2">
         <v>7</v>

</xml_diff>